<commit_message>
added a date field
</commit_message>
<xml_diff>
--- a/health_tracker/uploads/peter_data_2019.xlsx
+++ b/health_tracker/uploads/peter_data_2019.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,300 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>43711.36360478804</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>45</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>43711.36394776197</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>45</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>43711.36485364258</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>43711.36509579796</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>43711.36578422158</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>meditation</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>43711</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>45</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed datepicker error messaging
</commit_message>
<xml_diff>
--- a/health_tracker/uploads/peter_data_2019.xlsx
+++ b/health_tracker/uploads/peter_data_2019.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,153 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>43690</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>30</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>exercise</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>43740</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" t="n">
+        <v>15</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>work</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>43709</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>60</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>work</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added accurate error messaging for all fields
</commit_message>
<xml_diff>
--- a/health_tracker/uploads/peter_data_2019.xlsx
+++ b/health_tracker/uploads/peter_data_2019.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -922,6 +922,55 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>43723</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>30</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>meditation</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the issue with user entry dates overlapping
</commit_message>
<xml_diff>
--- a/health_tracker/uploads/peter_data_2019.xlsx
+++ b/health_tracker/uploads/peter_data_2019.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,14 +444,14 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>43732</v>
+        <v>43734</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -465,39 +465,39 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="G2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>meditation</t>
+          <t>looking at phone</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>43732</v>
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
         <v>12</v>
@@ -530,22 +530,234 @@
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
         <v>3</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
         <v>3</v>
       </c>
       <c r="O3" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>43732</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>meditation</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>43732</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>exercise</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>43732</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>looking at phone</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>43732</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>30</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>exercise</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>4</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>